<commit_message>
best vers with bugs
</commit_message>
<xml_diff>
--- a/Transport_task/data.xlsx
+++ b/Transport_task/data.xlsx
@@ -5,15 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serge\OneDrive\Desktop\bmstu\VKR\program\diploma\Transport_task\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serge\OneDrive\Desktop\bmstu\VKR\new_program\Tr_task\Transport_task\Transport_task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4076C81-27B8-4886-AE0D-C88223F33852}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1959D822-C7B4-496D-B294-3562DCC1AA79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10808" yWindow="1530" windowWidth="12510" windowHeight="12870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14595" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист3" sheetId="4" r:id="rId3"/>
+    <sheet name="Лист4" sheetId="5" r:id="rId4"/>
+    <sheet name="Лист5" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -55,8 +59,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -339,8 +344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -413,4 +418,1398 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF851F3-C2F7-43DD-9808-B94C6B442F25}">
+  <dimension ref="A2:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="A1:H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B2">
+        <v>150</v>
+      </c>
+      <c r="C2">
+        <v>130</v>
+      </c>
+      <c r="D2">
+        <v>150</v>
+      </c>
+      <c r="E2">
+        <v>140</v>
+      </c>
+      <c r="F2">
+        <v>45</v>
+      </c>
+      <c r="G2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>200</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>7</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>180</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>190</v>
+      </c>
+      <c r="B5">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>64</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>8</v>
+      </c>
+      <c r="G6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>48</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10BE3A23-EC6F-4276-8948-9344AC80C5EC}">
+  <dimension ref="A2:AJ32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="B2" s="1">
+        <v>130</v>
+      </c>
+      <c r="C2" s="1">
+        <v>150</v>
+      </c>
+      <c r="D2" s="1">
+        <v>140</v>
+      </c>
+      <c r="E2" s="1">
+        <v>45</v>
+      </c>
+      <c r="F2" s="1">
+        <v>67</v>
+      </c>
+      <c r="G2" s="1">
+        <v>120</v>
+      </c>
+      <c r="H2" s="1">
+        <v>130</v>
+      </c>
+      <c r="I2" s="1">
+        <v>178</v>
+      </c>
+      <c r="J2" s="1">
+        <v>150</v>
+      </c>
+      <c r="K2" s="1">
+        <v>130</v>
+      </c>
+      <c r="L2" s="1">
+        <v>150</v>
+      </c>
+      <c r="M2" s="1">
+        <v>140</v>
+      </c>
+      <c r="N2" s="1">
+        <v>45</v>
+      </c>
+      <c r="O2" s="1">
+        <v>67</v>
+      </c>
+      <c r="P2" s="1">
+        <v>120</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>130</v>
+      </c>
+      <c r="R2" s="1">
+        <v>178</v>
+      </c>
+      <c r="S2" s="1">
+        <v>150</v>
+      </c>
+      <c r="T2" s="1">
+        <v>130</v>
+      </c>
+      <c r="U2" s="1">
+        <v>150</v>
+      </c>
+      <c r="V2" s="1">
+        <v>140</v>
+      </c>
+      <c r="W2" s="1">
+        <v>45</v>
+      </c>
+      <c r="X2" s="1">
+        <v>67</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>120</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>130</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>178</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>150</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>130</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>150</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>140</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>45</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>67</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>120</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>130</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59D14104-FF9C-4DD5-AEB8-54126F1DFE80}">
+  <dimension ref="A2:L12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B2">
+        <v>150</v>
+      </c>
+      <c r="C2">
+        <v>130</v>
+      </c>
+      <c r="D2">
+        <v>150</v>
+      </c>
+      <c r="E2">
+        <v>140</v>
+      </c>
+      <c r="F2">
+        <v>45</v>
+      </c>
+      <c r="G2">
+        <v>67</v>
+      </c>
+      <c r="H2">
+        <v>100</v>
+      </c>
+      <c r="I2">
+        <v>70</v>
+      </c>
+      <c r="J2">
+        <v>90</v>
+      </c>
+      <c r="K2">
+        <v>150</v>
+      </c>
+      <c r="L2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>200</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>7</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>180</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>190</v>
+      </c>
+      <c r="B5">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>64</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>8</v>
+      </c>
+      <c r="G6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>48</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F04A415-6434-4A4B-96BA-9AC09E93D2C5}">
+  <dimension ref="A2:DB92"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="J87" sqref="J87"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="2" spans="1:106" x14ac:dyDescent="0.45">
+      <c r="B2" s="1">
+        <v>130</v>
+      </c>
+      <c r="C2" s="1">
+        <v>150</v>
+      </c>
+      <c r="D2" s="1">
+        <v>140</v>
+      </c>
+      <c r="E2" s="1">
+        <v>45</v>
+      </c>
+      <c r="F2" s="1">
+        <v>67</v>
+      </c>
+      <c r="G2" s="1">
+        <v>120</v>
+      </c>
+      <c r="H2" s="1">
+        <v>130</v>
+      </c>
+      <c r="I2" s="1">
+        <v>178</v>
+      </c>
+      <c r="J2" s="1">
+        <v>150</v>
+      </c>
+      <c r="K2" s="1">
+        <v>130</v>
+      </c>
+      <c r="L2" s="1">
+        <v>150</v>
+      </c>
+      <c r="M2" s="1">
+        <v>140</v>
+      </c>
+      <c r="N2" s="1">
+        <v>45</v>
+      </c>
+      <c r="O2" s="1">
+        <v>67</v>
+      </c>
+      <c r="P2" s="1">
+        <v>120</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>130</v>
+      </c>
+      <c r="R2" s="1">
+        <v>178</v>
+      </c>
+      <c r="S2" s="1">
+        <v>150</v>
+      </c>
+      <c r="T2" s="1">
+        <v>130</v>
+      </c>
+      <c r="U2" s="1">
+        <v>150</v>
+      </c>
+      <c r="V2" s="1">
+        <v>140</v>
+      </c>
+      <c r="W2" s="1">
+        <v>45</v>
+      </c>
+      <c r="X2" s="1">
+        <v>67</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>120</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>130</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>178</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>150</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>130</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>150</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>140</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>45</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>67</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>120</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>130</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>178</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>130</v>
+      </c>
+      <c r="AL2" s="1">
+        <v>150</v>
+      </c>
+      <c r="AM2" s="1">
+        <v>140</v>
+      </c>
+      <c r="AN2" s="1">
+        <v>45</v>
+      </c>
+      <c r="AO2" s="1">
+        <v>67</v>
+      </c>
+      <c r="AP2" s="1">
+        <v>120</v>
+      </c>
+      <c r="AQ2" s="1">
+        <v>130</v>
+      </c>
+      <c r="AR2" s="1">
+        <v>178</v>
+      </c>
+      <c r="AS2" s="1">
+        <v>150</v>
+      </c>
+      <c r="AT2" s="1">
+        <v>130</v>
+      </c>
+      <c r="AU2" s="1">
+        <v>150</v>
+      </c>
+      <c r="AV2" s="1">
+        <v>140</v>
+      </c>
+      <c r="AW2" s="1">
+        <v>45</v>
+      </c>
+      <c r="AX2" s="1">
+        <v>67</v>
+      </c>
+      <c r="AY2" s="1">
+        <v>120</v>
+      </c>
+      <c r="AZ2" s="1">
+        <v>130</v>
+      </c>
+      <c r="BA2" s="1">
+        <v>178</v>
+      </c>
+      <c r="BB2" s="1">
+        <v>150</v>
+      </c>
+      <c r="BC2" s="1">
+        <v>130</v>
+      </c>
+      <c r="BD2" s="1">
+        <v>150</v>
+      </c>
+      <c r="BE2" s="1">
+        <v>140</v>
+      </c>
+      <c r="BF2" s="1">
+        <v>45</v>
+      </c>
+      <c r="BG2" s="1">
+        <v>67</v>
+      </c>
+      <c r="BH2" s="1">
+        <v>120</v>
+      </c>
+      <c r="BI2" s="1">
+        <v>130</v>
+      </c>
+      <c r="BJ2" s="1">
+        <v>178</v>
+      </c>
+      <c r="BK2" s="1">
+        <v>150</v>
+      </c>
+      <c r="BL2" s="1">
+        <v>130</v>
+      </c>
+      <c r="BM2" s="1">
+        <v>150</v>
+      </c>
+      <c r="BN2" s="1">
+        <v>140</v>
+      </c>
+      <c r="BO2" s="1">
+        <v>45</v>
+      </c>
+      <c r="BP2" s="1">
+        <v>67</v>
+      </c>
+      <c r="BQ2" s="1">
+        <v>120</v>
+      </c>
+      <c r="BR2" s="1">
+        <v>130</v>
+      </c>
+      <c r="BS2" s="1">
+        <v>178</v>
+      </c>
+      <c r="BT2" s="1">
+        <v>130</v>
+      </c>
+      <c r="BU2" s="1">
+        <v>150</v>
+      </c>
+      <c r="BV2" s="1">
+        <v>140</v>
+      </c>
+      <c r="BW2" s="1">
+        <v>45</v>
+      </c>
+      <c r="BX2" s="1">
+        <v>67</v>
+      </c>
+      <c r="BY2" s="1">
+        <v>120</v>
+      </c>
+      <c r="BZ2" s="1">
+        <v>130</v>
+      </c>
+      <c r="CA2" s="1">
+        <v>178</v>
+      </c>
+      <c r="CB2" s="1">
+        <v>150</v>
+      </c>
+      <c r="CC2" s="1">
+        <v>130</v>
+      </c>
+      <c r="CD2" s="1">
+        <v>150</v>
+      </c>
+      <c r="CE2" s="1">
+        <v>140</v>
+      </c>
+      <c r="CF2" s="1">
+        <v>45</v>
+      </c>
+      <c r="CG2" s="1">
+        <v>67</v>
+      </c>
+      <c r="CH2" s="1">
+        <v>120</v>
+      </c>
+      <c r="CI2" s="1">
+        <v>130</v>
+      </c>
+      <c r="CJ2" s="1">
+        <v>178</v>
+      </c>
+      <c r="CK2" s="1">
+        <v>150</v>
+      </c>
+      <c r="CL2" s="1">
+        <v>130</v>
+      </c>
+      <c r="CM2" s="1">
+        <v>150</v>
+      </c>
+      <c r="CN2" s="1">
+        <v>140</v>
+      </c>
+      <c r="CO2" s="1">
+        <v>45</v>
+      </c>
+      <c r="CP2" s="1">
+        <v>67</v>
+      </c>
+      <c r="CQ2" s="1">
+        <v>120</v>
+      </c>
+      <c r="CR2" s="1">
+        <v>130</v>
+      </c>
+      <c r="CS2" s="1">
+        <v>178</v>
+      </c>
+      <c r="CT2" s="1">
+        <v>150</v>
+      </c>
+      <c r="CU2" s="1">
+        <v>130</v>
+      </c>
+      <c r="CV2" s="1">
+        <v>150</v>
+      </c>
+      <c r="CW2" s="1">
+        <v>140</v>
+      </c>
+      <c r="CX2" s="1">
+        <v>45</v>
+      </c>
+      <c r="CY2" s="1">
+        <v>67</v>
+      </c>
+      <c r="CZ2" s="1">
+        <v>120</v>
+      </c>
+      <c r="DA2" s="1">
+        <v>130</v>
+      </c>
+      <c r="DB2" s="1">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:106" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:106" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:106" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:106" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:106" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:106" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:106" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:106" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:106" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:106" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:106" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:106" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="15" spans="1:106" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="16" spans="1:106" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A56">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A57">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A58">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A59">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A60">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A61">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A62">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A63">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A64">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A66">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A67">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A68">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A69">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A70">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A71">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A72">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A73">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A74">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A75">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A76">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A77">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A78">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A79">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A80">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A81">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A82">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A83">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A84">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A85">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A86">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A87">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A88">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A89">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A90">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A91">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A92">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>